<commit_message>
Corrected Degraders list v4
</commit_message>
<xml_diff>
--- a/Degraders_list_v4.xlsx
+++ b/Degraders_list_v4.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20475" uniqueCount="2160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20475" uniqueCount="2159">
   <si>
     <t xml:space="preserve">Microorganism</t>
   </si>
@@ -6065,9 +6065,6 @@
   </si>
   <si>
     <t xml:space="preserve">The biodegradable polymer used in this study consisted of fine particles of poly caprolactone (PCL) with the trade TM name PLACCEL H7 (Daicel Chemical Industries Ltd Tokio). The molecular weight of the PCL was c. 70 000 and the diameter of the PCL particles ranged from 63 to 250 mm.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Streptomyces thermoolivaceous</t>
   </si>
   <si>
     <t xml:space="preserve">Streptomyces thermoviolaceus</t>
@@ -6650,8 +6647,8 @@
   </sheetPr>
   <dimension ref="A1:S1204"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1110" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1117" activeCellId="0" sqref="B1117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -71859,7 +71856,7 @@
     </row>
     <row r="1106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1106" s="9" t="s">
-        <v>2015</v>
+        <v>1961</v>
       </c>
       <c r="B1106" s="2" t="n">
         <v>0</v>
@@ -71918,7 +71915,7 @@
     </row>
     <row r="1107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1107" s="4" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B1107" s="2" t="n">
         <v>0</v>
@@ -71927,19 +71924,19 @@
         <v>64</v>
       </c>
       <c r="D1107" s="4" t="s">
+        <v>2016</v>
+      </c>
+      <c r="E1107" s="3" t="s">
         <v>2017</v>
       </c>
-      <c r="E1107" s="3" t="s">
+      <c r="F1107" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1107" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1107" s="3" t="s">
         <v>2018</v>
-      </c>
-      <c r="F1107" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1107" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1107" s="3" t="s">
-        <v>2019</v>
       </c>
       <c r="I1107" s="3" t="n">
         <v>2013</v>
@@ -71948,7 +71945,7 @@
         <v>83</v>
       </c>
       <c r="K1107" s="5" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="L1107" s="5" t="s">
         <v>23</v>
@@ -71977,7 +71974,7 @@
     </row>
     <row r="1108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1108" s="9" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="B1108" s="2" t="n">
         <v>0</v>
@@ -72036,10 +72033,10 @@
     </row>
     <row r="1109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1109" s="4" t="s">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B1109" s="2" t="n">
-        <v>0</v>
+        <v>67581</v>
       </c>
       <c r="C1109" s="2" t="s">
         <v>1450</v>
@@ -72095,10 +72092,10 @@
     </row>
     <row r="1110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1110" s="7" t="s">
-        <v>2022</v>
-      </c>
-      <c r="B1110" s="8" t="n">
-        <v>0</v>
+        <v>2021</v>
+      </c>
+      <c r="B1110" s="2" t="n">
+        <v>67581</v>
       </c>
       <c r="C1110" s="8" t="s">
         <v>113</v>
@@ -72154,10 +72151,10 @@
     </row>
     <row r="1111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1111" s="4" t="s">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="B1111" s="2" t="n">
-        <v>0</v>
+        <v>28572</v>
       </c>
       <c r="C1111" s="2" t="s">
         <v>64</v>
@@ -72213,16 +72210,16 @@
     </row>
     <row r="1112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1112" s="4" t="s">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="B1112" s="2" t="n">
-        <v>0</v>
+        <v>28572</v>
       </c>
       <c r="C1112" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D1112" s="4" t="s">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="E1112" s="3" t="s">
         <v>1279</v>
@@ -72272,16 +72269,16 @@
     </row>
     <row r="1113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1113" s="4" t="s">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="B1113" s="2" t="n">
-        <v>0</v>
+        <v>28572</v>
       </c>
       <c r="C1113" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D1113" s="4" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="E1113" s="3" t="s">
         <v>1279</v>
@@ -72331,10 +72328,10 @@
     </row>
     <row r="1114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1114" s="4" t="s">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="B1114" s="2" t="n">
-        <v>0</v>
+        <v>28572</v>
       </c>
       <c r="C1114" s="2" t="s">
         <v>64</v>
@@ -72343,7 +72340,7 @@
         <v>1744</v>
       </c>
       <c r="E1114" s="3" t="s">
-        <v>2026</v>
+        <v>2025</v>
       </c>
       <c r="F1114" s="3" t="s">
         <v>22</v>
@@ -72361,7 +72358,7 @@
         <v>581</v>
       </c>
       <c r="K1114" s="5" t="s">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="L1114" s="5" t="s">
         <v>126</v>
@@ -72390,10 +72387,10 @@
     </row>
     <row r="1115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1115" s="4" t="s">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="B1115" s="2" t="n">
-        <v>0</v>
+        <v>28572</v>
       </c>
       <c r="C1115" s="2" t="s">
         <v>20</v>
@@ -72402,7 +72399,7 @@
         <v>1744</v>
       </c>
       <c r="E1115" s="3" t="s">
-        <v>2026</v>
+        <v>2025</v>
       </c>
       <c r="F1115" s="3" t="s">
         <v>22</v>
@@ -72420,7 +72417,7 @@
         <v>581</v>
       </c>
       <c r="K1115" s="5" t="s">
-        <v>2028</v>
+        <v>2027</v>
       </c>
       <c r="L1115" s="5" t="s">
         <v>185</v>
@@ -72449,10 +72446,10 @@
     </row>
     <row r="1116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1116" s="4" t="s">
-        <v>2029</v>
+        <v>2028</v>
       </c>
       <c r="B1116" s="2" t="n">
-        <v>0</v>
+        <v>28574</v>
       </c>
       <c r="C1116" s="2" t="s">
         <v>20</v>
@@ -72508,7 +72505,7 @@
     </row>
     <row r="1117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1117" s="4" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
       <c r="B1117" s="2" t="n">
         <v>0</v>
@@ -72567,7 +72564,7 @@
     </row>
     <row r="1118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1118" s="4" t="s">
-        <v>2031</v>
+        <v>2030</v>
       </c>
       <c r="B1118" s="2" t="n">
         <v>0</v>
@@ -72576,7 +72573,7 @@
         <v>237</v>
       </c>
       <c r="D1118" s="4" t="s">
-        <v>2032</v>
+        <v>2031</v>
       </c>
       <c r="E1118" s="3" t="s">
         <v>22</v>
@@ -72594,10 +72591,10 @@
         <v>2017</v>
       </c>
       <c r="J1118" s="5" t="s">
+        <v>2032</v>
+      </c>
+      <c r="K1118" s="5" t="s">
         <v>2033</v>
-      </c>
-      <c r="K1118" s="5" t="s">
-        <v>2034</v>
       </c>
       <c r="L1118" s="5" t="s">
         <v>185</v>
@@ -72626,7 +72623,7 @@
     </row>
     <row r="1119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1119" s="4" t="s">
-        <v>2035</v>
+        <v>2034</v>
       </c>
       <c r="B1119" s="2" t="n">
         <v>0</v>
@@ -72685,7 +72682,7 @@
     </row>
     <row r="1120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1120" s="4" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="B1120" s="2" t="n">
         <v>0</v>
@@ -72744,7 +72741,7 @@
     </row>
     <row r="1121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1121" s="4" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="B1121" s="2" t="n">
         <v>0</v>
@@ -72803,7 +72800,7 @@
     </row>
     <row r="1122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1122" s="4" t="s">
-        <v>2038</v>
+        <v>2037</v>
       </c>
       <c r="B1122" s="2" t="n">
         <v>0</v>
@@ -72862,7 +72859,7 @@
     </row>
     <row r="1123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1123" s="4" t="s">
-        <v>2039</v>
+        <v>2038</v>
       </c>
       <c r="B1123" s="2" t="n">
         <v>0</v>
@@ -72921,7 +72918,7 @@
     </row>
     <row r="1124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1124" s="7" t="s">
-        <v>2039</v>
+        <v>2038</v>
       </c>
       <c r="B1124" s="8" t="n">
         <v>0</v>
@@ -72951,7 +72948,7 @@
         <v>441</v>
       </c>
       <c r="K1124" s="5" t="s">
-        <v>2040</v>
+        <v>2039</v>
       </c>
       <c r="L1124" s="5" t="s">
         <v>62</v>
@@ -72980,7 +72977,7 @@
     </row>
     <row r="1125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1125" s="4" t="s">
-        <v>2039</v>
+        <v>2038</v>
       </c>
       <c r="B1125" s="2" t="n">
         <v>0</v>
@@ -73039,7 +73036,7 @@
     </row>
     <row r="1126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1126" s="9" t="s">
-        <v>2041</v>
+        <v>2040</v>
       </c>
       <c r="B1126" s="2" t="n">
         <v>0</v>
@@ -73057,10 +73054,10 @@
         <v>39</v>
       </c>
       <c r="G1126" s="3" t="s">
+        <v>2041</v>
+      </c>
+      <c r="H1126" s="3" t="s">
         <v>2042</v>
-      </c>
-      <c r="H1126" s="3" t="s">
-        <v>2043</v>
       </c>
       <c r="I1126" s="3" t="s">
         <v>23</v>
@@ -73098,7 +73095,7 @@
     </row>
     <row r="1127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1127" s="4" t="s">
-        <v>2041</v>
+        <v>2040</v>
       </c>
       <c r="B1127" s="2" t="n">
         <v>0</v>
@@ -73116,10 +73113,10 @@
         <v>39</v>
       </c>
       <c r="G1127" s="3" t="s">
+        <v>2043</v>
+      </c>
+      <c r="H1127" s="3" t="s">
         <v>2044</v>
-      </c>
-      <c r="H1127" s="3" t="s">
-        <v>2045</v>
       </c>
       <c r="I1127" s="3" t="n">
         <v>2010</v>
@@ -73157,7 +73154,7 @@
     </row>
     <row r="1128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1128" s="4" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
       <c r="B1128" s="2" t="n">
         <v>0</v>
@@ -73166,7 +73163,7 @@
         <v>108</v>
       </c>
       <c r="D1128" s="4" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="E1128" s="3" t="s">
         <v>492</v>
@@ -73175,19 +73172,19 @@
         <v>39</v>
       </c>
       <c r="G1128" s="3" t="s">
+        <v>2047</v>
+      </c>
+      <c r="H1128" s="3" t="s">
         <v>2048</v>
-      </c>
-      <c r="H1128" s="3" t="s">
-        <v>2049</v>
       </c>
       <c r="I1128" s="3" t="n">
         <v>2011</v>
       </c>
       <c r="J1128" s="5" t="s">
+        <v>2049</v>
+      </c>
+      <c r="K1128" s="6" t="s">
         <v>2050</v>
-      </c>
-      <c r="K1128" s="6" t="s">
-        <v>2051</v>
       </c>
       <c r="L1128" s="5" t="s">
         <v>185</v>
@@ -73216,7 +73213,7 @@
     </row>
     <row r="1129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1129" s="4" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
       <c r="B1129" s="2" t="n">
         <v>0</v>
@@ -73225,7 +73222,7 @@
         <v>108</v>
       </c>
       <c r="D1129" s="4" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="E1129" s="3" t="s">
         <v>492</v>
@@ -73234,19 +73231,19 @@
         <v>39</v>
       </c>
       <c r="G1129" s="3" t="s">
+        <v>2051</v>
+      </c>
+      <c r="H1129" s="3" t="s">
         <v>2052</v>
-      </c>
-      <c r="H1129" s="3" t="s">
-        <v>2053</v>
       </c>
       <c r="I1129" s="3" t="n">
         <v>2011</v>
       </c>
       <c r="J1129" s="5" t="s">
+        <v>2049</v>
+      </c>
+      <c r="K1129" s="6" t="s">
         <v>2050</v>
-      </c>
-      <c r="K1129" s="6" t="s">
-        <v>2051</v>
       </c>
       <c r="L1129" s="5" t="s">
         <v>185</v>
@@ -73275,7 +73272,7 @@
     </row>
     <row r="1130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1130" s="4" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
       <c r="B1130" s="2" t="n">
         <v>0</v>
@@ -73334,7 +73331,7 @@
     </row>
     <row r="1131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1131" s="4" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
       <c r="B1131" s="2" t="n">
         <v>0</v>
@@ -73393,7 +73390,7 @@
     </row>
     <row r="1132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1132" s="9" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
       <c r="B1132" s="2" t="n">
         <v>0</v>
@@ -73411,10 +73408,10 @@
         <v>39</v>
       </c>
       <c r="G1132" s="3" t="s">
+        <v>2054</v>
+      </c>
+      <c r="H1132" s="3" t="s">
         <v>2055</v>
-      </c>
-      <c r="H1132" s="3" t="s">
-        <v>2056</v>
       </c>
       <c r="I1132" s="3" t="s">
         <v>23</v>
@@ -73452,7 +73449,7 @@
     </row>
     <row r="1133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1133" s="4" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
       <c r="B1133" s="2" t="n">
         <v>0</v>
@@ -73461,7 +73458,7 @@
         <v>108</v>
       </c>
       <c r="D1133" s="4" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="E1133" s="3" t="s">
         <v>492</v>
@@ -73470,19 +73467,19 @@
         <v>39</v>
       </c>
       <c r="G1133" s="3" t="s">
+        <v>2056</v>
+      </c>
+      <c r="H1133" s="3" t="s">
         <v>2057</v>
-      </c>
-      <c r="H1133" s="3" t="s">
-        <v>2058</v>
       </c>
       <c r="I1133" s="3" t="n">
         <v>2011</v>
       </c>
       <c r="J1133" s="5" t="s">
+        <v>2049</v>
+      </c>
+      <c r="K1133" s="6" t="s">
         <v>2050</v>
-      </c>
-      <c r="K1133" s="6" t="s">
-        <v>2051</v>
       </c>
       <c r="L1133" s="5" t="s">
         <v>185</v>
@@ -73511,7 +73508,7 @@
     </row>
     <row r="1134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1134" s="4" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
       <c r="B1134" s="2" t="n">
         <v>0</v>
@@ -73570,16 +73567,16 @@
     </row>
     <row r="1135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1135" s="4" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
       <c r="B1135" s="2" t="n">
         <v>0</v>
       </c>
       <c r="C1135" s="2" t="s">
+        <v>2058</v>
+      </c>
+      <c r="D1135" s="4" t="s">
         <v>2059</v>
-      </c>
-      <c r="D1135" s="4" t="s">
-        <v>2060</v>
       </c>
       <c r="E1135" s="3" t="s">
         <v>22</v>
@@ -73600,7 +73597,7 @@
         <v>75</v>
       </c>
       <c r="K1135" s="5" t="s">
-        <v>2061</v>
+        <v>2060</v>
       </c>
       <c r="L1135" s="5" t="s">
         <v>23</v>
@@ -73629,7 +73626,7 @@
     </row>
     <row r="1136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1136" s="4" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
       <c r="B1136" s="2" t="n">
         <v>0</v>
@@ -73638,7 +73635,7 @@
         <v>108</v>
       </c>
       <c r="D1136" s="4" t="s">
-        <v>2062</v>
+        <v>2061</v>
       </c>
       <c r="E1136" s="3" t="s">
         <v>492</v>
@@ -73688,7 +73685,7 @@
     </row>
     <row r="1137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1137" s="4" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
       <c r="B1137" s="3" t="n">
         <v>0</v>
@@ -73700,16 +73697,16 @@
         <v>1267</v>
       </c>
       <c r="E1137" s="3" t="s">
+        <v>2063</v>
+      </c>
+      <c r="F1137" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1137" s="3" t="s">
         <v>2064</v>
       </c>
-      <c r="F1137" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1137" s="3" t="s">
+      <c r="H1137" s="3" t="s">
         <v>2065</v>
-      </c>
-      <c r="H1137" s="3" t="s">
-        <v>2066</v>
       </c>
       <c r="I1137" s="3" t="s">
         <v>23</v>
@@ -73747,7 +73744,7 @@
     </row>
     <row r="1138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1138" s="4" t="s">
-        <v>2067</v>
+        <v>2066</v>
       </c>
       <c r="B1138" s="3" t="n">
         <v>0</v>
@@ -73765,10 +73762,10 @@
         <v>39</v>
       </c>
       <c r="G1138" s="3" t="s">
+        <v>2067</v>
+      </c>
+      <c r="H1138" s="3" t="s">
         <v>2068</v>
-      </c>
-      <c r="H1138" s="3" t="s">
-        <v>2069</v>
       </c>
       <c r="I1138" s="3" t="s">
         <v>23</v>
@@ -73806,7 +73803,7 @@
     </row>
     <row r="1139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1139" s="4" t="s">
-        <v>2070</v>
+        <v>2069</v>
       </c>
       <c r="B1139" s="2" t="n">
         <v>0</v>
@@ -73865,7 +73862,7 @@
     </row>
     <row r="1140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1140" s="4" t="s">
-        <v>2071</v>
+        <v>2070</v>
       </c>
       <c r="B1140" s="2" t="n">
         <v>0</v>
@@ -73924,7 +73921,7 @@
     </row>
     <row r="1141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1141" s="4" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
       <c r="B1141" s="2" t="n">
         <v>0</v>
@@ -73933,7 +73930,7 @@
         <v>30</v>
       </c>
       <c r="D1141" s="4" t="s">
-        <v>2073</v>
+        <v>2072</v>
       </c>
       <c r="E1141" s="3" t="s">
         <v>22</v>
@@ -73951,10 +73948,10 @@
         <v>2014</v>
       </c>
       <c r="J1141" s="5" t="s">
+        <v>2073</v>
+      </c>
+      <c r="K1141" s="6" t="s">
         <v>2074</v>
-      </c>
-      <c r="K1141" s="6" t="s">
-        <v>2075</v>
       </c>
       <c r="L1141" s="5" t="s">
         <v>314</v>
@@ -73972,7 +73969,7 @@
         <v>158</v>
       </c>
       <c r="Q1141" s="5" t="s">
-        <v>2076</v>
+        <v>2075</v>
       </c>
       <c r="R1141" s="5" t="s">
         <v>39</v>
@@ -73983,7 +73980,7 @@
     </row>
     <row r="1142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1142" s="4" t="s">
-        <v>2077</v>
+        <v>2076</v>
       </c>
       <c r="B1142" s="2" t="n">
         <v>0</v>
@@ -74042,7 +74039,7 @@
     </row>
     <row r="1143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1143" s="4" t="s">
-        <v>2078</v>
+        <v>2077</v>
       </c>
       <c r="B1143" s="2" t="n">
         <v>0</v>
@@ -74101,7 +74098,7 @@
     </row>
     <row r="1144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1144" s="4" t="s">
-        <v>2079</v>
+        <v>2078</v>
       </c>
       <c r="B1144" s="2" t="n">
         <v>0</v>
@@ -74160,7 +74157,7 @@
     </row>
     <row r="1145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1145" s="4" t="s">
-        <v>2079</v>
+        <v>2078</v>
       </c>
       <c r="B1145" s="2" t="n">
         <v>0</v>
@@ -74219,7 +74216,7 @@
     </row>
     <row r="1146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1146" s="4" t="s">
-        <v>2079</v>
+        <v>2078</v>
       </c>
       <c r="B1146" s="2" t="n">
         <v>0</v>
@@ -74278,7 +74275,7 @@
     </row>
     <row r="1147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1147" s="4" t="s">
-        <v>2079</v>
+        <v>2078</v>
       </c>
       <c r="B1147" s="2" t="n">
         <v>0</v>
@@ -74337,7 +74334,7 @@
     </row>
     <row r="1148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1148" s="4" t="s">
-        <v>2079</v>
+        <v>2078</v>
       </c>
       <c r="B1148" s="2" t="n">
         <v>0</v>
@@ -74346,10 +74343,10 @@
         <v>113</v>
       </c>
       <c r="D1148" s="4" t="s">
+        <v>2079</v>
+      </c>
+      <c r="E1148" s="3" t="s">
         <v>2080</v>
-      </c>
-      <c r="E1148" s="3" t="s">
-        <v>2081</v>
       </c>
       <c r="F1148" s="3" t="s">
         <v>22</v>
@@ -74364,10 +74361,10 @@
         <v>2014</v>
       </c>
       <c r="J1148" s="5" t="s">
+        <v>2081</v>
+      </c>
+      <c r="K1148" s="5" t="s">
         <v>2082</v>
-      </c>
-      <c r="K1148" s="5" t="s">
-        <v>2083</v>
       </c>
       <c r="L1148" s="5" t="s">
         <v>23</v>
@@ -74396,7 +74393,7 @@
     </row>
     <row r="1149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1149" s="4" t="s">
-        <v>2079</v>
+        <v>2078</v>
       </c>
       <c r="B1149" s="2" t="n">
         <v>0</v>
@@ -74455,7 +74452,7 @@
     </row>
     <row r="1150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1150" s="4" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
       <c r="B1150" s="2" t="n">
         <v>0</v>
@@ -74514,7 +74511,7 @@
     </row>
     <row r="1151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1151" s="4" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
       <c r="B1151" s="2" t="n">
         <v>0</v>
@@ -74523,7 +74520,7 @@
         <v>134</v>
       </c>
       <c r="D1151" s="4" t="s">
-        <v>2085</v>
+        <v>2084</v>
       </c>
       <c r="E1151" s="3" t="s">
         <v>22</v>
@@ -74544,10 +74541,10 @@
         <v>83</v>
       </c>
       <c r="K1151" s="5" t="s">
+        <v>2085</v>
+      </c>
+      <c r="L1151" s="5" t="s">
         <v>2086</v>
-      </c>
-      <c r="L1151" s="5" t="s">
-        <v>2087</v>
       </c>
       <c r="M1151" s="5" t="s">
         <v>27</v>
@@ -74573,7 +74570,7 @@
     </row>
     <row r="1152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1152" s="4" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
       <c r="B1152" s="2" t="n">
         <v>0</v>
@@ -74632,7 +74629,7 @@
     </row>
     <row r="1153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1153" s="9" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
       <c r="B1153" s="2" t="n">
         <v>0</v>
@@ -74691,7 +74688,7 @@
     </row>
     <row r="1154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1154" s="4" t="s">
-        <v>2088</v>
+        <v>2087</v>
       </c>
       <c r="B1154" s="2" t="n">
         <v>0</v>
@@ -74718,7 +74715,7 @@
         <v>2004</v>
       </c>
       <c r="J1154" s="5" t="s">
-        <v>2089</v>
+        <v>2088</v>
       </c>
       <c r="K1154" s="5" t="s">
         <v>470</v>
@@ -74750,7 +74747,7 @@
     </row>
     <row r="1155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1155" s="4" t="s">
-        <v>2090</v>
+        <v>2089</v>
       </c>
       <c r="B1155" s="2" t="n">
         <v>0</v>
@@ -74759,7 +74756,7 @@
         <v>30</v>
       </c>
       <c r="D1155" s="4" t="s">
-        <v>2091</v>
+        <v>2090</v>
       </c>
       <c r="E1155" s="3" t="s">
         <v>22</v>
@@ -74777,10 +74774,10 @@
         <v>2016</v>
       </c>
       <c r="J1155" s="5" t="s">
+        <v>2091</v>
+      </c>
+      <c r="K1155" s="5" t="s">
         <v>2092</v>
-      </c>
-      <c r="K1155" s="5" t="s">
-        <v>2093</v>
       </c>
       <c r="L1155" s="5" t="s">
         <v>314</v>
@@ -74809,7 +74806,7 @@
     </row>
     <row r="1156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1156" s="4" t="s">
-        <v>2090</v>
+        <v>2089</v>
       </c>
       <c r="B1156" s="2" t="n">
         <v>0</v>
@@ -74868,7 +74865,7 @@
     </row>
     <row r="1157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1157" s="4" t="s">
-        <v>2094</v>
+        <v>2093</v>
       </c>
       <c r="B1157" s="2" t="n">
         <v>0</v>
@@ -74927,7 +74924,7 @@
     </row>
     <row r="1158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1158" s="4" t="s">
-        <v>2095</v>
+        <v>2094</v>
       </c>
       <c r="B1158" s="2" t="n">
         <v>1914427</v>
@@ -74986,7 +74983,7 @@
     </row>
     <row r="1159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1159" s="9" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B1159" s="2" t="n">
         <v>0</v>
@@ -75004,10 +75001,10 @@
         <v>39</v>
       </c>
       <c r="G1159" s="3" t="s">
+        <v>2096</v>
+      </c>
+      <c r="H1159" s="3" t="s">
         <v>2097</v>
-      </c>
-      <c r="H1159" s="3" t="s">
-        <v>2098</v>
       </c>
       <c r="I1159" s="3" t="n">
         <v>2018</v>
@@ -75045,7 +75042,7 @@
     </row>
     <row r="1160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1160" s="9" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B1160" s="2" t="n">
         <v>0</v>
@@ -75063,10 +75060,10 @@
         <v>39</v>
       </c>
       <c r="G1160" s="3" t="s">
+        <v>2096</v>
+      </c>
+      <c r="H1160" s="3" t="s">
         <v>2097</v>
-      </c>
-      <c r="H1160" s="3" t="s">
-        <v>2098</v>
       </c>
       <c r="I1160" s="3" t="n">
         <v>2018</v>
@@ -75104,7 +75101,7 @@
     </row>
     <row r="1161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1161" s="4" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B1161" s="2" t="n">
         <v>0</v>
@@ -75113,7 +75110,7 @@
         <v>30</v>
       </c>
       <c r="D1161" s="4" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="E1161" s="3" t="s">
         <v>1291</v>
@@ -75122,10 +75119,10 @@
         <v>39</v>
       </c>
       <c r="G1161" s="3" t="s">
+        <v>2099</v>
+      </c>
+      <c r="H1161" s="3" t="s">
         <v>2100</v>
-      </c>
-      <c r="H1161" s="3" t="s">
-        <v>2101</v>
       </c>
       <c r="I1161" s="3" t="n">
         <v>2008</v>
@@ -75134,7 +75131,7 @@
         <v>92</v>
       </c>
       <c r="K1161" s="6" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="L1161" s="5" t="s">
         <v>984</v>
@@ -75163,7 +75160,7 @@
     </row>
     <row r="1162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1162" s="4" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B1162" s="2" t="n">
         <v>0</v>
@@ -75172,7 +75169,7 @@
         <v>30</v>
       </c>
       <c r="D1162" s="4" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="E1162" s="3" t="s">
         <v>1291</v>
@@ -75181,10 +75178,10 @@
         <v>39</v>
       </c>
       <c r="G1162" s="3" t="s">
+        <v>2102</v>
+      </c>
+      <c r="H1162" s="3" t="s">
         <v>2103</v>
-      </c>
-      <c r="H1162" s="3" t="s">
-        <v>2104</v>
       </c>
       <c r="I1162" s="3" t="n">
         <v>2008</v>
@@ -75193,7 +75190,7 @@
         <v>92</v>
       </c>
       <c r="K1162" s="6" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="L1162" s="5" t="s">
         <v>984</v>
@@ -75222,7 +75219,7 @@
     </row>
     <row r="1163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1163" s="4" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B1163" s="2" t="n">
         <v>0</v>
@@ -75231,7 +75228,7 @@
         <v>30</v>
       </c>
       <c r="D1163" s="4" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="E1163" s="3" t="s">
         <v>1291</v>
@@ -75240,10 +75237,10 @@
         <v>39</v>
       </c>
       <c r="G1163" s="3" t="s">
+        <v>2104</v>
+      </c>
+      <c r="H1163" s="3" t="s">
         <v>2105</v>
-      </c>
-      <c r="H1163" s="3" t="s">
-        <v>2106</v>
       </c>
       <c r="I1163" s="3" t="n">
         <v>2008</v>
@@ -75252,7 +75249,7 @@
         <v>92</v>
       </c>
       <c r="K1163" s="6" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="L1163" s="5" t="s">
         <v>984</v>
@@ -75281,7 +75278,7 @@
     </row>
     <row r="1164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1164" s="4" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B1164" s="2" t="n">
         <v>0</v>
@@ -75290,7 +75287,7 @@
         <v>30</v>
       </c>
       <c r="D1164" s="4" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="E1164" s="3" t="s">
         <v>1291</v>
@@ -75299,10 +75296,10 @@
         <v>39</v>
       </c>
       <c r="G1164" s="3" t="s">
+        <v>2106</v>
+      </c>
+      <c r="H1164" s="3" t="s">
         <v>2107</v>
-      </c>
-      <c r="H1164" s="3" t="s">
-        <v>2108</v>
       </c>
       <c r="I1164" s="3" t="n">
         <v>2008</v>
@@ -75311,7 +75308,7 @@
         <v>92</v>
       </c>
       <c r="K1164" s="6" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="L1164" s="5" t="s">
         <v>984</v>
@@ -75340,7 +75337,7 @@
     </row>
     <row r="1165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1165" s="4" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B1165" s="2" t="n">
         <v>0</v>
@@ -75349,7 +75346,7 @@
         <v>30</v>
       </c>
       <c r="D1165" s="4" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="E1165" s="3" t="s">
         <v>1291</v>
@@ -75358,10 +75355,10 @@
         <v>39</v>
       </c>
       <c r="G1165" s="3" t="s">
+        <v>2108</v>
+      </c>
+      <c r="H1165" s="3" t="s">
         <v>2109</v>
-      </c>
-      <c r="H1165" s="3" t="s">
-        <v>2110</v>
       </c>
       <c r="I1165" s="3" t="n">
         <v>2008</v>
@@ -75370,7 +75367,7 @@
         <v>92</v>
       </c>
       <c r="K1165" s="6" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="L1165" s="5" t="s">
         <v>984</v>
@@ -75399,7 +75396,7 @@
     </row>
     <row r="1166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1166" s="4" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B1166" s="2" t="n">
         <v>0</v>
@@ -75408,7 +75405,7 @@
         <v>374</v>
       </c>
       <c r="D1166" s="4" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="E1166" s="3" t="s">
         <v>1291</v>
@@ -75417,10 +75414,10 @@
         <v>39</v>
       </c>
       <c r="G1166" s="3" t="s">
+        <v>2099</v>
+      </c>
+      <c r="H1166" s="3" t="s">
         <v>2100</v>
-      </c>
-      <c r="H1166" s="3" t="s">
-        <v>2101</v>
       </c>
       <c r="I1166" s="3" t="n">
         <v>2008</v>
@@ -75429,7 +75426,7 @@
         <v>216</v>
       </c>
       <c r="K1166" s="6" t="s">
-        <v>2111</v>
+        <v>2110</v>
       </c>
       <c r="L1166" s="5" t="s">
         <v>100</v>
@@ -75458,7 +75455,7 @@
     </row>
     <row r="1167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1167" s="4" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B1167" s="2" t="n">
         <v>0</v>
@@ -75467,7 +75464,7 @@
         <v>374</v>
       </c>
       <c r="D1167" s="4" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="E1167" s="3" t="s">
         <v>1291</v>
@@ -75476,10 +75473,10 @@
         <v>39</v>
       </c>
       <c r="G1167" s="3" t="s">
+        <v>2104</v>
+      </c>
+      <c r="H1167" s="3" t="s">
         <v>2105</v>
-      </c>
-      <c r="H1167" s="3" t="s">
-        <v>2106</v>
       </c>
       <c r="I1167" s="3" t="n">
         <v>2008</v>
@@ -75488,7 +75485,7 @@
         <v>216</v>
       </c>
       <c r="K1167" s="6" t="s">
-        <v>2111</v>
+        <v>2110</v>
       </c>
       <c r="L1167" s="5" t="s">
         <v>100</v>
@@ -75517,7 +75514,7 @@
     </row>
     <row r="1168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1168" s="4" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B1168" s="2" t="n">
         <v>0</v>
@@ -75526,7 +75523,7 @@
         <v>374</v>
       </c>
       <c r="D1168" s="4" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="E1168" s="3" t="s">
         <v>1291</v>
@@ -75535,10 +75532,10 @@
         <v>39</v>
       </c>
       <c r="G1168" s="3" t="s">
+        <v>2108</v>
+      </c>
+      <c r="H1168" s="3" t="s">
         <v>2109</v>
-      </c>
-      <c r="H1168" s="3" t="s">
-        <v>2110</v>
       </c>
       <c r="I1168" s="3" t="n">
         <v>2008</v>
@@ -75547,7 +75544,7 @@
         <v>216</v>
       </c>
       <c r="K1168" s="6" t="s">
-        <v>2111</v>
+        <v>2110</v>
       </c>
       <c r="L1168" s="5" t="s">
         <v>100</v>
@@ -75576,7 +75573,7 @@
     </row>
     <row r="1169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1169" s="4" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B1169" s="2" t="n">
         <v>0</v>
@@ -75585,7 +75582,7 @@
         <v>78</v>
       </c>
       <c r="D1169" s="4" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="E1169" s="3" t="s">
         <v>1291</v>
@@ -75594,10 +75591,10 @@
         <v>39</v>
       </c>
       <c r="G1169" s="3" t="s">
+        <v>2099</v>
+      </c>
+      <c r="H1169" s="3" t="s">
         <v>2100</v>
-      </c>
-      <c r="H1169" s="3" t="s">
-        <v>2101</v>
       </c>
       <c r="I1169" s="3" t="n">
         <v>2008</v>
@@ -75606,7 +75603,7 @@
         <v>216</v>
       </c>
       <c r="K1169" s="6" t="s">
-        <v>2112</v>
+        <v>2111</v>
       </c>
       <c r="L1169" s="5" t="s">
         <v>62</v>
@@ -75635,7 +75632,7 @@
     </row>
     <row r="1170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1170" s="4" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B1170" s="2" t="n">
         <v>0</v>
@@ -75644,7 +75641,7 @@
         <v>58</v>
       </c>
       <c r="D1170" s="4" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="E1170" s="3" t="s">
         <v>1291</v>
@@ -75653,10 +75650,10 @@
         <v>39</v>
       </c>
       <c r="G1170" s="3" t="s">
+        <v>2099</v>
+      </c>
+      <c r="H1170" s="3" t="s">
         <v>2100</v>
-      </c>
-      <c r="H1170" s="3" t="s">
-        <v>2101</v>
       </c>
       <c r="I1170" s="3" t="n">
         <v>2008</v>
@@ -75665,7 +75662,7 @@
         <v>216</v>
       </c>
       <c r="K1170" s="6" t="s">
-        <v>2112</v>
+        <v>2111</v>
       </c>
       <c r="L1170" s="5" t="s">
         <v>62</v>
@@ -75694,7 +75691,7 @@
     </row>
     <row r="1171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1171" s="4" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B1171" s="2" t="n">
         <v>0</v>
@@ -75703,7 +75700,7 @@
         <v>78</v>
       </c>
       <c r="D1171" s="4" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="E1171" s="3" t="s">
         <v>1291</v>
@@ -75712,10 +75709,10 @@
         <v>39</v>
       </c>
       <c r="G1171" s="3" t="s">
+        <v>2104</v>
+      </c>
+      <c r="H1171" s="3" t="s">
         <v>2105</v>
-      </c>
-      <c r="H1171" s="3" t="s">
-        <v>2106</v>
       </c>
       <c r="I1171" s="3" t="n">
         <v>2008</v>
@@ -75724,7 +75721,7 @@
         <v>216</v>
       </c>
       <c r="K1171" s="6" t="s">
-        <v>2112</v>
+        <v>2111</v>
       </c>
       <c r="L1171" s="5" t="s">
         <v>62</v>
@@ -75753,7 +75750,7 @@
     </row>
     <row r="1172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1172" s="7" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B1172" s="8" t="n">
         <v>0</v>
@@ -75762,7 +75759,7 @@
         <v>58</v>
       </c>
       <c r="D1172" s="7" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="E1172" s="5" t="s">
         <v>1291</v>
@@ -75771,10 +75768,10 @@
         <v>39</v>
       </c>
       <c r="G1172" s="5" t="s">
+        <v>2104</v>
+      </c>
+      <c r="H1172" s="5" t="s">
         <v>2105</v>
-      </c>
-      <c r="H1172" s="5" t="s">
-        <v>2106</v>
       </c>
       <c r="I1172" s="5" t="n">
         <v>2008</v>
@@ -75783,7 +75780,7 @@
         <v>216</v>
       </c>
       <c r="K1172" s="6" t="s">
-        <v>2112</v>
+        <v>2111</v>
       </c>
       <c r="L1172" s="5" t="s">
         <v>62</v>
@@ -75812,7 +75809,7 @@
     </row>
     <row r="1173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1173" s="4" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B1173" s="2" t="n">
         <v>0</v>
@@ -75821,7 +75818,7 @@
         <v>78</v>
       </c>
       <c r="D1173" s="4" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="E1173" s="3" t="s">
         <v>1291</v>
@@ -75830,10 +75827,10 @@
         <v>39</v>
       </c>
       <c r="G1173" s="3" t="s">
+        <v>2108</v>
+      </c>
+      <c r="H1173" s="3" t="s">
         <v>2109</v>
-      </c>
-      <c r="H1173" s="3" t="s">
-        <v>2110</v>
       </c>
       <c r="I1173" s="3" t="n">
         <v>2008</v>
@@ -75842,7 +75839,7 @@
         <v>216</v>
       </c>
       <c r="K1173" s="6" t="s">
-        <v>2112</v>
+        <v>2111</v>
       </c>
       <c r="L1173" s="5" t="s">
         <v>62</v>
@@ -75871,7 +75868,7 @@
     </row>
     <row r="1174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1174" s="4" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B1174" s="2" t="n">
         <v>0</v>
@@ -75880,7 +75877,7 @@
         <v>58</v>
       </c>
       <c r="D1174" s="4" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="E1174" s="3" t="s">
         <v>1291</v>
@@ -75889,10 +75886,10 @@
         <v>39</v>
       </c>
       <c r="G1174" s="3" t="s">
+        <v>2108</v>
+      </c>
+      <c r="H1174" s="3" t="s">
         <v>2109</v>
-      </c>
-      <c r="H1174" s="3" t="s">
-        <v>2110</v>
       </c>
       <c r="I1174" s="3" t="n">
         <v>2008</v>
@@ -75901,7 +75898,7 @@
         <v>216</v>
       </c>
       <c r="K1174" s="6" t="s">
-        <v>2112</v>
+        <v>2111</v>
       </c>
       <c r="L1174" s="5" t="s">
         <v>62</v>
@@ -75930,7 +75927,7 @@
     </row>
     <row r="1175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1175" s="4" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B1175" s="2" t="n">
         <v>0</v>
@@ -75939,7 +75936,7 @@
         <v>20</v>
       </c>
       <c r="D1175" s="4" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="E1175" s="3" t="s">
         <v>1291</v>
@@ -75948,10 +75945,10 @@
         <v>39</v>
       </c>
       <c r="G1175" s="3" t="s">
+        <v>2099</v>
+      </c>
+      <c r="H1175" s="3" t="s">
         <v>2100</v>
-      </c>
-      <c r="H1175" s="3" t="s">
-        <v>2101</v>
       </c>
       <c r="I1175" s="3" t="n">
         <v>2008</v>
@@ -75960,7 +75957,7 @@
         <v>216</v>
       </c>
       <c r="K1175" s="6" t="s">
-        <v>2113</v>
+        <v>2112</v>
       </c>
       <c r="L1175" s="5" t="s">
         <v>185</v>
@@ -75989,7 +75986,7 @@
     </row>
     <row r="1176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1176" s="4" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B1176" s="2" t="n">
         <v>0</v>
@@ -75998,7 +75995,7 @@
         <v>20</v>
       </c>
       <c r="D1176" s="4" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="E1176" s="3" t="s">
         <v>1291</v>
@@ -76007,10 +76004,10 @@
         <v>39</v>
       </c>
       <c r="G1176" s="3" t="s">
+        <v>2104</v>
+      </c>
+      <c r="H1176" s="3" t="s">
         <v>2105</v>
-      </c>
-      <c r="H1176" s="3" t="s">
-        <v>2106</v>
       </c>
       <c r="I1176" s="3" t="n">
         <v>2008</v>
@@ -76019,7 +76016,7 @@
         <v>216</v>
       </c>
       <c r="K1176" s="6" t="s">
-        <v>2113</v>
+        <v>2112</v>
       </c>
       <c r="L1176" s="5" t="s">
         <v>185</v>
@@ -76048,7 +76045,7 @@
     </row>
     <row r="1177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1177" s="4" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B1177" s="2" t="n">
         <v>0</v>
@@ -76057,7 +76054,7 @@
         <v>64</v>
       </c>
       <c r="D1177" s="4" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="E1177" s="3" t="s">
         <v>1291</v>
@@ -76066,10 +76063,10 @@
         <v>39</v>
       </c>
       <c r="G1177" s="3" t="s">
+        <v>2099</v>
+      </c>
+      <c r="H1177" s="3" t="s">
         <v>2100</v>
-      </c>
-      <c r="H1177" s="3" t="s">
-        <v>2101</v>
       </c>
       <c r="I1177" s="3" t="n">
         <v>2008</v>
@@ -76078,7 +76075,7 @@
         <v>216</v>
       </c>
       <c r="K1177" s="6" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="L1177" s="5" t="s">
         <v>984</v>
@@ -76107,7 +76104,7 @@
     </row>
     <row r="1178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1178" s="4" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B1178" s="2" t="n">
         <v>0</v>
@@ -76116,7 +76113,7 @@
         <v>64</v>
       </c>
       <c r="D1178" s="4" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="E1178" s="3" t="s">
         <v>1291</v>
@@ -76125,10 +76122,10 @@
         <v>39</v>
       </c>
       <c r="G1178" s="3" t="s">
+        <v>2104</v>
+      </c>
+      <c r="H1178" s="3" t="s">
         <v>2105</v>
-      </c>
-      <c r="H1178" s="3" t="s">
-        <v>2106</v>
       </c>
       <c r="I1178" s="3" t="n">
         <v>2008</v>
@@ -76137,7 +76134,7 @@
         <v>216</v>
       </c>
       <c r="K1178" s="6" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="L1178" s="5" t="s">
         <v>984</v>
@@ -76166,7 +76163,7 @@
     </row>
     <row r="1179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1179" s="4" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B1179" s="2" t="n">
         <v>0</v>
@@ -76175,7 +76172,7 @@
         <v>64</v>
       </c>
       <c r="D1179" s="4" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="E1179" s="3" t="s">
         <v>1291</v>
@@ -76184,10 +76181,10 @@
         <v>39</v>
       </c>
       <c r="G1179" s="3" t="s">
+        <v>2108</v>
+      </c>
+      <c r="H1179" s="3" t="s">
         <v>2109</v>
-      </c>
-      <c r="H1179" s="3" t="s">
-        <v>2110</v>
       </c>
       <c r="I1179" s="3" t="n">
         <v>2008</v>
@@ -76196,7 +76193,7 @@
         <v>216</v>
       </c>
       <c r="K1179" s="6" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="L1179" s="5" t="s">
         <v>984</v>
@@ -76225,7 +76222,7 @@
     </row>
     <row r="1180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1180" s="4" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B1180" s="2" t="n">
         <v>0</v>
@@ -76234,19 +76231,19 @@
         <v>677</v>
       </c>
       <c r="D1180" s="4" t="s">
+        <v>2113</v>
+      </c>
+      <c r="E1180" s="3" t="s">
         <v>2114</v>
       </c>
-      <c r="E1180" s="3" t="s">
+      <c r="F1180" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1180" s="3" t="s">
         <v>2115</v>
       </c>
-      <c r="F1180" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1180" s="3" t="s">
+      <c r="H1180" s="3" t="s">
         <v>2116</v>
-      </c>
-      <c r="H1180" s="3" t="s">
-        <v>2117</v>
       </c>
       <c r="I1180" s="3" t="n">
         <v>2017</v>
@@ -76255,7 +76252,7 @@
         <v>1190</v>
       </c>
       <c r="K1180" s="6" t="s">
-        <v>2118</v>
+        <v>2117</v>
       </c>
       <c r="L1180" s="5" t="s">
         <v>682</v>
@@ -76284,7 +76281,7 @@
     </row>
     <row r="1181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1181" s="4" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B1181" s="2" t="n">
         <v>0</v>
@@ -76293,19 +76290,19 @@
         <v>677</v>
       </c>
       <c r="D1181" s="4" t="s">
+        <v>2113</v>
+      </c>
+      <c r="E1181" s="3" t="s">
         <v>2114</v>
       </c>
-      <c r="E1181" s="3" t="s">
-        <v>2115</v>
-      </c>
       <c r="F1181" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G1181" s="3" t="s">
+        <v>2118</v>
+      </c>
+      <c r="H1181" s="3" t="s">
         <v>2119</v>
-      </c>
-      <c r="H1181" s="3" t="s">
-        <v>2120</v>
       </c>
       <c r="I1181" s="3" t="n">
         <v>2017</v>
@@ -76314,7 +76311,7 @@
         <v>1190</v>
       </c>
       <c r="K1181" s="6" t="s">
-        <v>2118</v>
+        <v>2117</v>
       </c>
       <c r="L1181" s="5" t="s">
         <v>682</v>
@@ -76343,7 +76340,7 @@
     </row>
     <row r="1182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1182" s="4" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B1182" s="2" t="n">
         <v>0</v>
@@ -76352,19 +76349,19 @@
         <v>677</v>
       </c>
       <c r="D1182" s="4" t="s">
+        <v>2113</v>
+      </c>
+      <c r="E1182" s="3" t="s">
         <v>2114</v>
       </c>
-      <c r="E1182" s="3" t="s">
-        <v>2115</v>
-      </c>
       <c r="F1182" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G1182" s="3" t="s">
+        <v>2120</v>
+      </c>
+      <c r="H1182" s="3" t="s">
         <v>2121</v>
-      </c>
-      <c r="H1182" s="3" t="s">
-        <v>2122</v>
       </c>
       <c r="I1182" s="3" t="n">
         <v>2017</v>
@@ -76373,7 +76370,7 @@
         <v>1190</v>
       </c>
       <c r="K1182" s="6" t="s">
-        <v>2118</v>
+        <v>2117</v>
       </c>
       <c r="L1182" s="5" t="s">
         <v>682</v>
@@ -76402,7 +76399,7 @@
     </row>
     <row r="1183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1183" s="4" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B1183" s="2" t="n">
         <v>0</v>
@@ -76411,19 +76408,19 @@
         <v>677</v>
       </c>
       <c r="D1183" s="4" t="s">
+        <v>2113</v>
+      </c>
+      <c r="E1183" s="3" t="s">
         <v>2114</v>
       </c>
-      <c r="E1183" s="3" t="s">
-        <v>2115</v>
-      </c>
       <c r="F1183" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G1183" s="3" t="s">
+        <v>2122</v>
+      </c>
+      <c r="H1183" s="10" t="s">
         <v>2123</v>
-      </c>
-      <c r="H1183" s="10" t="s">
-        <v>2124</v>
       </c>
       <c r="I1183" s="3" t="n">
         <v>2017</v>
@@ -76432,7 +76429,7 @@
         <v>1190</v>
       </c>
       <c r="K1183" s="6" t="s">
-        <v>2118</v>
+        <v>2117</v>
       </c>
       <c r="L1183" s="5" t="s">
         <v>682</v>
@@ -76461,7 +76458,7 @@
     </row>
     <row r="1184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1184" s="4" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B1184" s="2" t="n">
         <v>0</v>
@@ -76470,19 +76467,19 @@
         <v>677</v>
       </c>
       <c r="D1184" s="4" t="s">
+        <v>2113</v>
+      </c>
+      <c r="E1184" s="3" t="s">
         <v>2114</v>
       </c>
-      <c r="E1184" s="3" t="s">
-        <v>2115</v>
-      </c>
       <c r="F1184" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G1184" s="3" t="s">
+        <v>2124</v>
+      </c>
+      <c r="H1184" s="3" t="s">
         <v>2125</v>
-      </c>
-      <c r="H1184" s="3" t="s">
-        <v>2126</v>
       </c>
       <c r="I1184" s="3" t="n">
         <v>2017</v>
@@ -76491,7 +76488,7 @@
         <v>1190</v>
       </c>
       <c r="K1184" s="6" t="s">
-        <v>2118</v>
+        <v>2117</v>
       </c>
       <c r="L1184" s="5" t="s">
         <v>682</v>
@@ -76520,7 +76517,7 @@
     </row>
     <row r="1185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1185" s="4" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B1185" s="2" t="n">
         <v>0</v>
@@ -76529,19 +76526,19 @@
         <v>677</v>
       </c>
       <c r="D1185" s="4" t="s">
+        <v>2113</v>
+      </c>
+      <c r="E1185" s="3" t="s">
         <v>2114</v>
       </c>
-      <c r="E1185" s="3" t="s">
-        <v>2115</v>
-      </c>
       <c r="F1185" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G1185" s="3" t="s">
+        <v>2126</v>
+      </c>
+      <c r="H1185" s="3" t="s">
         <v>2127</v>
-      </c>
-      <c r="H1185" s="3" t="s">
-        <v>2128</v>
       </c>
       <c r="I1185" s="3" t="n">
         <v>2017</v>
@@ -76550,7 +76547,7 @@
         <v>1190</v>
       </c>
       <c r="K1185" s="6" t="s">
-        <v>2118</v>
+        <v>2117</v>
       </c>
       <c r="L1185" s="5" t="s">
         <v>682</v>
@@ -76579,7 +76576,7 @@
     </row>
     <row r="1186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1186" s="4" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B1186" s="2" t="n">
         <v>0</v>
@@ -76588,7 +76585,7 @@
         <v>108</v>
       </c>
       <c r="D1186" s="4" t="s">
-        <v>2129</v>
+        <v>2128</v>
       </c>
       <c r="E1186" s="3" t="s">
         <v>492</v>
@@ -76597,10 +76594,10 @@
         <v>39</v>
       </c>
       <c r="G1186" s="3" t="s">
+        <v>2129</v>
+      </c>
+      <c r="H1186" s="3" t="s">
         <v>2130</v>
-      </c>
-      <c r="H1186" s="3" t="s">
-        <v>2131</v>
       </c>
       <c r="I1186" s="3" t="n">
         <v>2012</v>
@@ -76609,7 +76606,7 @@
         <v>75</v>
       </c>
       <c r="K1186" s="10" t="s">
-        <v>2132</v>
+        <v>2131</v>
       </c>
       <c r="L1186" s="3" t="s">
         <v>23</v>
@@ -76638,7 +76635,7 @@
     </row>
     <row r="1187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1187" s="4" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B1187" s="2" t="n">
         <v>0</v>
@@ -76647,7 +76644,7 @@
         <v>64</v>
       </c>
       <c r="D1187" s="4" t="s">
-        <v>2129</v>
+        <v>2128</v>
       </c>
       <c r="E1187" s="3" t="s">
         <v>492</v>
@@ -76656,10 +76653,10 @@
         <v>39</v>
       </c>
       <c r="G1187" s="3" t="s">
+        <v>2129</v>
+      </c>
+      <c r="H1187" s="3" t="s">
         <v>2130</v>
-      </c>
-      <c r="H1187" s="3" t="s">
-        <v>2131</v>
       </c>
       <c r="I1187" s="3" t="n">
         <v>2012</v>
@@ -76668,7 +76665,7 @@
         <v>75</v>
       </c>
       <c r="K1187" s="10" t="s">
-        <v>2133</v>
+        <v>2132</v>
       </c>
       <c r="L1187" s="5" t="s">
         <v>984</v>
@@ -76697,7 +76694,7 @@
     </row>
     <row r="1188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1188" s="4" t="s">
-        <v>2134</v>
+        <v>2133</v>
       </c>
       <c r="B1188" s="2" t="n">
         <v>0</v>
@@ -76756,7 +76753,7 @@
     </row>
     <row r="1189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1189" s="7" t="s">
-        <v>2135</v>
+        <v>2134</v>
       </c>
       <c r="B1189" s="8" t="n">
         <v>0</v>
@@ -76786,7 +76783,7 @@
         <v>60</v>
       </c>
       <c r="K1189" s="5" t="s">
-        <v>2136</v>
+        <v>2135</v>
       </c>
       <c r="L1189" s="5" t="s">
         <v>439</v>
@@ -76815,7 +76812,7 @@
     </row>
     <row r="1190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1190" s="4" t="s">
-        <v>2135</v>
+        <v>2134</v>
       </c>
       <c r="B1190" s="2" t="n">
         <v>0</v>
@@ -76845,7 +76842,7 @@
         <v>60</v>
       </c>
       <c r="K1190" s="5" t="s">
-        <v>2137</v>
+        <v>2136</v>
       </c>
       <c r="L1190" s="5" t="s">
         <v>439</v>
@@ -76874,7 +76871,7 @@
     </row>
     <row r="1191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1191" s="4" t="s">
-        <v>2135</v>
+        <v>2134</v>
       </c>
       <c r="B1191" s="2" t="n">
         <v>0</v>
@@ -76933,7 +76930,7 @@
     </row>
     <row r="1192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1192" s="4" t="s">
-        <v>2135</v>
+        <v>2134</v>
       </c>
       <c r="B1192" s="2" t="n">
         <v>0</v>
@@ -76992,7 +76989,7 @@
     </row>
     <row r="1193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1193" s="4" t="s">
-        <v>2135</v>
+        <v>2134</v>
       </c>
       <c r="B1193" s="2" t="n">
         <v>0</v>
@@ -77051,7 +77048,7 @@
     </row>
     <row r="1194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1194" s="4" t="s">
-        <v>2135</v>
+        <v>2134</v>
       </c>
       <c r="B1194" s="2" t="n">
         <v>0</v>
@@ -77110,16 +77107,16 @@
     </row>
     <row r="1195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1195" s="4" t="s">
+        <v>2137</v>
+      </c>
+      <c r="B1195" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1195" s="2" t="s">
         <v>2138</v>
       </c>
-      <c r="B1195" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C1195" s="2" t="s">
+      <c r="D1195" s="4" t="s">
         <v>2139</v>
-      </c>
-      <c r="D1195" s="4" t="s">
-        <v>2140</v>
       </c>
       <c r="E1195" s="3" t="s">
         <v>22</v>
@@ -77137,10 +77134,10 @@
         <v>2015</v>
       </c>
       <c r="J1195" s="5" t="s">
+        <v>2140</v>
+      </c>
+      <c r="K1195" s="5" t="s">
         <v>2141</v>
-      </c>
-      <c r="K1195" s="5" t="s">
-        <v>2142</v>
       </c>
       <c r="L1195" s="5" t="s">
         <v>1026</v>
@@ -77169,16 +77166,16 @@
     </row>
     <row r="1196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1196" s="4" t="s">
-        <v>2138</v>
+        <v>2137</v>
       </c>
       <c r="B1196" s="2" t="n">
         <v>0</v>
       </c>
       <c r="C1196" s="2" t="s">
-        <v>2143</v>
+        <v>2142</v>
       </c>
       <c r="D1196" s="4" t="s">
-        <v>2140</v>
+        <v>2139</v>
       </c>
       <c r="E1196" s="3" t="s">
         <v>22</v>
@@ -77196,13 +77193,13 @@
         <v>2014</v>
       </c>
       <c r="J1196" s="5" t="s">
-        <v>2141</v>
+        <v>2140</v>
       </c>
       <c r="K1196" s="5" t="s">
+        <v>2143</v>
+      </c>
+      <c r="L1196" s="5" t="s">
         <v>2144</v>
-      </c>
-      <c r="L1196" s="5" t="s">
-        <v>2145</v>
       </c>
       <c r="M1196" s="5" t="s">
         <v>27</v>
@@ -77228,7 +77225,7 @@
     </row>
     <row r="1197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1197" s="4" t="s">
-        <v>2146</v>
+        <v>2145</v>
       </c>
       <c r="B1197" s="2" t="n">
         <v>29494</v>
@@ -77287,7 +77284,7 @@
     </row>
     <row r="1198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1198" s="9" t="s">
-        <v>2147</v>
+        <v>2146</v>
       </c>
       <c r="B1198" s="2" t="n">
         <v>0</v>
@@ -77305,10 +77302,10 @@
         <v>39</v>
       </c>
       <c r="G1198" s="3" t="s">
+        <v>2147</v>
+      </c>
+      <c r="H1198" s="3" t="s">
         <v>2148</v>
-      </c>
-      <c r="H1198" s="3" t="s">
-        <v>2149</v>
       </c>
       <c r="I1198" s="3" t="n">
         <v>2018</v>
@@ -77346,7 +77343,7 @@
     </row>
     <row r="1199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1199" s="9" t="s">
-        <v>2147</v>
+        <v>2146</v>
       </c>
       <c r="B1199" s="2" t="n">
         <v>0</v>
@@ -77364,10 +77361,10 @@
         <v>39</v>
       </c>
       <c r="G1199" s="3" t="s">
+        <v>2147</v>
+      </c>
+      <c r="H1199" s="3" t="s">
         <v>2148</v>
-      </c>
-      <c r="H1199" s="3" t="s">
-        <v>2149</v>
       </c>
       <c r="I1199" s="3" t="n">
         <v>2018</v>
@@ -77405,16 +77402,16 @@
     </row>
     <row r="1200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1200" s="4" t="s">
-        <v>2150</v>
+        <v>2149</v>
       </c>
       <c r="B1200" s="2" t="n">
         <v>0</v>
       </c>
       <c r="C1200" s="2" t="s">
+        <v>2138</v>
+      </c>
+      <c r="D1200" s="4" t="s">
         <v>2139</v>
-      </c>
-      <c r="D1200" s="4" t="s">
-        <v>2140</v>
       </c>
       <c r="E1200" s="3" t="s">
         <v>22</v>
@@ -77432,10 +77429,10 @@
         <v>2017</v>
       </c>
       <c r="J1200" s="5" t="s">
+        <v>2140</v>
+      </c>
+      <c r="K1200" s="5" t="s">
         <v>2141</v>
-      </c>
-      <c r="K1200" s="5" t="s">
-        <v>2142</v>
       </c>
       <c r="L1200" s="5" t="s">
         <v>1026</v>
@@ -77464,16 +77461,16 @@
     </row>
     <row r="1201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1201" s="4" t="s">
-        <v>2150</v>
+        <v>2149</v>
       </c>
       <c r="B1201" s="2" t="n">
         <v>0</v>
       </c>
       <c r="C1201" s="2" t="s">
-        <v>2143</v>
+        <v>2142</v>
       </c>
       <c r="D1201" s="4" t="s">
-        <v>2140</v>
+        <v>2139</v>
       </c>
       <c r="E1201" s="3" t="s">
         <v>22</v>
@@ -77491,13 +77488,13 @@
         <v>2016</v>
       </c>
       <c r="J1201" s="5" t="s">
-        <v>2141</v>
+        <v>2140</v>
       </c>
       <c r="K1201" s="5" t="s">
+        <v>2143</v>
+      </c>
+      <c r="L1201" s="5" t="s">
         <v>2144</v>
-      </c>
-      <c r="L1201" s="5" t="s">
-        <v>2145</v>
       </c>
       <c r="M1201" s="5" t="s">
         <v>27</v>
@@ -77523,7 +77520,7 @@
     </row>
     <row r="1202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1202" s="4" t="s">
-        <v>2151</v>
+        <v>2150</v>
       </c>
       <c r="B1202" s="2" t="n">
         <v>0</v>
@@ -77582,7 +77579,7 @@
     </row>
     <row r="1203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1203" s="4" t="s">
-        <v>2152</v>
+        <v>2151</v>
       </c>
       <c r="B1203" s="2" t="n">
         <v>0</v>
@@ -77591,7 +77588,7 @@
         <v>113</v>
       </c>
       <c r="D1203" s="4" t="s">
-        <v>2153</v>
+        <v>2152</v>
       </c>
       <c r="E1203" s="3" t="s">
         <v>22</v>
@@ -77609,10 +77606,10 @@
         <v>2008</v>
       </c>
       <c r="J1203" s="5" t="s">
+        <v>2153</v>
+      </c>
+      <c r="K1203" s="5" t="s">
         <v>2154</v>
-      </c>
-      <c r="K1203" s="5" t="s">
-        <v>2155</v>
       </c>
       <c r="L1203" s="5" t="s">
         <v>23</v>
@@ -77641,7 +77638,7 @@
     </row>
     <row r="1204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1204" s="7" t="s">
-        <v>2156</v>
+        <v>2155</v>
       </c>
       <c r="B1204" s="8" t="n">
         <v>0</v>
@@ -77650,10 +77647,10 @@
         <v>1541</v>
       </c>
       <c r="D1204" s="7" t="s">
+        <v>2156</v>
+      </c>
+      <c r="E1204" s="5" t="s">
         <v>2157</v>
-      </c>
-      <c r="E1204" s="5" t="s">
-        <v>2158</v>
       </c>
       <c r="F1204" s="5" t="s">
         <v>22</v>
@@ -77671,7 +77668,7 @@
         <v>83</v>
       </c>
       <c r="K1204" s="5" t="s">
-        <v>2159</v>
+        <v>2158</v>
       </c>
       <c r="L1204" s="5" t="s">
         <v>23</v>

</xml_diff>